<commit_message>
colors added and fixed bugs
</commit_message>
<xml_diff>
--- a/B_plan_data.xlsx
+++ b/B_plan_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGG\Dropbox\Github\Vestergaard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832B102E-B0B7-4E3D-89C8-FCCC5A968219}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2732D8A4-C78A-4C7D-AEFD-6529CEAAFFCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{DAAE4708-AB0F-478A-8CE9-929A85F3F5BE}"/>
+    <workbookView xWindow="390" yWindow="0" windowWidth="20130" windowHeight="13080" xr2:uid="{DAAE4708-AB0F-478A-8CE9-929A85F3F5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 GF overhead is possible but not sure how easily calculated.</t>
       </text>
     </comment>
-    <comment ref="B19" authorId="3" shapeId="0" xr:uid="{95AC5C7A-72F9-4AB6-ACF3-420FFE158935}">
+    <comment ref="B18" authorId="3" shapeId="0" xr:uid="{95AC5C7A-72F9-4AB6-ACF3-420FFE158935}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -86,7 +86,7 @@
     percentage of nets remaining from what we started with</t>
       </text>
     </comment>
-    <comment ref="C19" authorId="4" shapeId="0" xr:uid="{F35AEA93-E158-45EB-BCC7-28BB4885736B}">
+    <comment ref="C18" authorId="4" shapeId="0" xr:uid="{F35AEA93-E158-45EB-BCC7-28BB4885736B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -94,7 +94,7 @@
     This is the number of nets that are effectively used</t>
       </text>
     </comment>
-    <comment ref="C20" authorId="5" shapeId="0" xr:uid="{CFF4D34E-CA36-4C0C-A93B-B182786004B2}">
+    <comment ref="C19" authorId="5" shapeId="0" xr:uid="{CFF4D34E-CA36-4C0C-A93B-B182786004B2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -102,7 +102,7 @@
     value of the nets efficiently used</t>
       </text>
     </comment>
-    <comment ref="B21" authorId="6" shapeId="0" xr:uid="{E955DB73-E97F-4C4E-9295-80864E311EDD}">
+    <comment ref="B20" authorId="6" shapeId="0" xr:uid="{E955DB73-E97F-4C4E-9295-80864E311EDD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -142,29 +142,6 @@
   </si>
   <si>
     <t xml:space="preserve">Number of effecive LLIN </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Degradation value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-(Insecticide + wear and tear)
-We are assuming that they are mutually exclusive</t>
-    </r>
   </si>
   <si>
     <r>
@@ -199,9 +176,6 @@
     <t>Lost value (all nets)</t>
   </si>
   <si>
-    <t>Reduce loss by 20%</t>
-  </si>
-  <si>
     <t xml:space="preserve">Improve use by 20% </t>
   </si>
   <si>
@@ -214,9 +188,6 @@
     <t>LLINs bought</t>
   </si>
   <si>
-    <t>ASP</t>
-  </si>
-  <si>
     <t xml:space="preserve">Market size </t>
   </si>
   <si>
@@ -233,6 +204,35 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Degradation value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+(Insecticide + wear and tear)
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduce loss by </t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -468,13 +468,6 @@
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -517,6 +510,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -861,16 +857,16 @@
     AMF overhead can be calculated from their website.
 GF overhead is possible but not sure how easily calculated.</text>
   </threadedComment>
-  <threadedComment ref="B19" dT="2020-03-25T14:43:01.21" personId="{AD0E29FA-D7A8-43DC-9865-5D1FF4E1063A}" id="{95AC5C7A-72F9-4AB6-ACF3-420FFE158935}">
+  <threadedComment ref="B18" dT="2020-03-25T14:43:01.21" personId="{AD0E29FA-D7A8-43DC-9865-5D1FF4E1063A}" id="{95AC5C7A-72F9-4AB6-ACF3-420FFE158935}">
     <text>percentage of nets remaining from what we started with</text>
   </threadedComment>
-  <threadedComment ref="C19" dT="2020-03-25T14:41:14.19" personId="{AD0E29FA-D7A8-43DC-9865-5D1FF4E1063A}" id="{F35AEA93-E158-45EB-BCC7-28BB4885736B}">
+  <threadedComment ref="C18" dT="2020-03-25T14:41:14.19" personId="{AD0E29FA-D7A8-43DC-9865-5D1FF4E1063A}" id="{F35AEA93-E158-45EB-BCC7-28BB4885736B}">
     <text>This is the number of nets that are effectively used</text>
   </threadedComment>
-  <threadedComment ref="C20" dT="2020-03-25T14:43:29.21" personId="{AD0E29FA-D7A8-43DC-9865-5D1FF4E1063A}" id="{CFF4D34E-CA36-4C0C-A93B-B182786004B2}">
+  <threadedComment ref="C19" dT="2020-03-25T14:43:29.21" personId="{AD0E29FA-D7A8-43DC-9865-5D1FF4E1063A}" id="{CFF4D34E-CA36-4C0C-A93B-B182786004B2}">
     <text>value of the nets efficiently used</text>
   </threadedComment>
-  <threadedComment ref="B21" dT="2020-03-25T14:44:42.03" personId="{AD0E29FA-D7A8-43DC-9865-5D1FF4E1063A}" id="{E955DB73-E97F-4C4E-9295-80864E311EDD}">
+  <threadedComment ref="B20" dT="2020-03-25T14:44:42.03" personId="{AD0E29FA-D7A8-43DC-9865-5D1FF4E1063A}" id="{E955DB73-E97F-4C4E-9295-80864E311EDD}">
     <text>percentage of value lost</text>
   </threadedComment>
 </ThreadedComments>
@@ -878,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39F588E-C6A6-449E-9F18-FF74BC1B1FFB}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -893,62 +889,62 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="C2" s="34">
+      <c r="C2" s="31">
         <v>211297998</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="35">
+      <c r="C3" s="32">
         <v>2.58</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2">
         <v>0.71</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="33">
         <f>C3*C2</f>
         <v>545148834.84000003</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38">
+        <v>18</v>
+      </c>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35">
         <v>636500000</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="39">
-        <v>0.1842</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="C6" s="36"/>
     </row>
     <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
@@ -994,11 +990,11 @@
         <v>94441277.021577463</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="37">
         <f>1-0.5692</f>
         <v>0.43079999999999996</v>
       </c>
@@ -1007,7 +1003,7 @@
         <v>40685302.140895568</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>5</v>
       </c>
@@ -1020,7 +1016,7 @@
         <v>2748241.1613279055</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
         <v>6</v>
       </c>
@@ -1032,7 +1028,7 @@
         <v>2606579.2457955377</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
         <v>7</v>
       </c>
@@ -1052,9 +1048,9 @@
         <v>82300570.221000016</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" ht="57" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B16" s="11">
         <f>B12+B13</f>
@@ -1067,7 +1063,7 @@
     </row>
     <row r="17" spans="1:3" ht="114" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="11">
         <f>B10+B11+B12+B13</f>
@@ -1078,87 +1074,88 @@
         <v>57656399.621673033</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-    </row>
-    <row r="19" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="21">
-        <f>C19/C2</f>
+    <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="18">
+        <f>C18/C2</f>
         <v>0.47128534587534399</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C18" s="19">
         <f>C2*(1-B10)*(1-B11)*(1-B12)*(1-B13)</f>
         <v>99581650.070197746</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="20" t="s">
+    <row r="19" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="20">
+        <f>B18</f>
+        <v>0.47128534587534399</v>
+      </c>
+      <c r="C19" s="21">
+        <f>B18*C9</f>
+        <v>361860080.53677493</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="23">
-        <f>B19</f>
-        <v>0.47128534587534399</v>
-      </c>
-      <c r="C20" s="24">
-        <f>B19*C9</f>
-        <v>361860080.53677493</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="21">
-        <f>C21/C9</f>
+      <c r="B20" s="18">
+        <f>C20/C9</f>
         <v>0.52871465412465601</v>
       </c>
+      <c r="C20" s="22">
+        <f>C9-C19</f>
+        <v>405955179.80125326</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="24">
+        <v>0.2</v>
+      </c>
       <c r="C21" s="25">
-        <f>C9-C20</f>
-        <v>405955179.80125326</v>
+        <f>C2*(1-0.8*B10)*(1-B11)*(1-B16)</f>
+        <v>102287840.79119085</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28">
-        <f>C2*(1-0.8*B10)*(1-B11)*(1-B16)</f>
-        <v>102287840.79119085</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="30">
+        <v>13</v>
+      </c>
+      <c r="B22" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="C22" s="27">
         <f>C2*(1-B10)*(1-0.8*B11)*(1-B16)</f>
         <v>114557820.02835573</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A24" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="30">
+    <row r="23" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="C23" s="27">
         <f>C2*(1-B10)*(1-B11)*(1-0.9*B16)</f>
         <v>100094992.23275086</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="33">
-        <f>SUM(C22:C24)</f>
+    <row r="24" spans="1:3" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30">
+        <f>SUM(C21:C23)</f>
         <v>316940653.05229747</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added cases and deaths
</commit_message>
<xml_diff>
--- a/B_plan_data.xlsx
+++ b/B_plan_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGG\Dropbox\Github\Vestergaard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20367B40-F75F-4341-B5DF-B7DDED2C0450}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8179B2-DB77-4627-A77B-176743151046}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22340" yWindow="1230" windowWidth="8360" windowHeight="15380" xr2:uid="{DAAE4708-AB0F-478A-8CE9-929A85F3F5BE}"/>
+    <workbookView xWindow="-19740" yWindow="-1120" windowWidth="17600" windowHeight="18470" xr2:uid="{DAAE4708-AB0F-478A-8CE9-929A85F3F5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>ITN MOP budget</t>
   </si>
@@ -234,9 +234,6 @@
     <t xml:space="preserve">Number of effective LLIN </t>
   </si>
   <si>
-    <t>% reduction in geographic coverage need</t>
-  </si>
-  <si>
     <t>Increase in value due to improved geographic coverage effectiveness</t>
   </si>
   <si>
@@ -247,6 +244,15 @@
   </si>
   <si>
     <t>Cost of distribution</t>
+  </si>
+  <si>
+    <t>Number of children deaths prevented</t>
+  </si>
+  <si>
+    <t>Number of malaria cases prevented</t>
+  </si>
+  <si>
+    <t>% Reduction in geographic coverage need</t>
   </si>
 </sst>
 </file>
@@ -488,7 +494,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -580,22 +586,10 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -608,6 +602,29 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="168" fontId="8" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="7" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -969,15 +986,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39F588E-C6A6-449E-9F18-FF74BC1B1FFB}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.46484375" customWidth="1"/>
+    <col min="1" max="1" width="36.46484375" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="20.796875" customWidth="1"/>
   </cols>
@@ -987,7 +1004,7 @@
         <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>14</v>
@@ -1046,14 +1063,14 @@
         <v>0</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="46">
+      <c r="C7" s="42">
         <f>0.18*C5</f>
         <v>114570000</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="47" t="s">
-        <v>30</v>
+      <c r="A8" s="43" t="s">
+        <v>29</v>
       </c>
       <c r="B8" s="2">
         <v>0.28999999999999998</v>
@@ -1076,7 +1093,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="44" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="6">
@@ -1088,7 +1105,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="44" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="8">
@@ -1101,8 +1118,8 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="48" t="s">
-        <v>29</v>
+      <c r="A12" s="44" t="s">
+        <v>28</v>
       </c>
       <c r="B12" s="9">
         <f>1-0.9709</f>
@@ -1114,7 +1131,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="44" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="9">
@@ -1126,7 +1143,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="44" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="9"/>
@@ -1136,7 +1153,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="44" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="9"/>
@@ -1166,7 +1183,7 @@
         <f>B10+B11+B12+B13</f>
         <v>0.61049999999999993</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="41">
         <f>B17*C$9</f>
         <v>468751216.43636614</v>
       </c>
@@ -1215,7 +1232,6 @@
         <v>0.2</v>
       </c>
       <c r="C21" s="30">
-        <f>C2*(1-((1-B21)*B10+B11+B12+B13))</f>
         <v>87498500.971799999</v>
       </c>
     </row>
@@ -1224,11 +1240,9 @@
         <v>16</v>
       </c>
       <c r="B22" s="15">
-        <f>C21/C2</f>
         <v>0.41410000000000002</v>
       </c>
       <c r="C22" s="31">
-        <f>B22*C9</f>
         <v>317952299.30597746</v>
       </c>
     </row>
@@ -1237,185 +1251,251 @@
         <v>17</v>
       </c>
       <c r="B23" s="33">
-        <f>1-B22</f>
         <v>0.58589999999999998</v>
       </c>
       <c r="C23" s="34">
-        <f>C9-C22</f>
         <v>449862961.03205073</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="36">
-        <v>0.2</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B24" s="36"/>
       <c r="C24" s="37">
-        <f>C2*(1-(B10+(1-B24)*B11+B12+B13))</f>
-        <v>100506005.72868</v>
+        <v>58216.824408959816</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="15">
-        <f>C24/C2</f>
-        <v>0.47565999999999997</v>
-      </c>
-      <c r="C25" s="31">
-        <f>B25*C9</f>
-        <v>365219006.73238647</v>
+        <v>31</v>
+      </c>
+      <c r="B25" s="15"/>
+      <c r="C25" s="45">
+        <v>1330670.2722047959</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="32" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B26" s="33">
-        <f>1-B25</f>
-        <v>0.52434000000000003</v>
-      </c>
-      <c r="C26" s="34">
-        <f>C9-C25</f>
-        <v>402596253.60564172</v>
+        <v>0.2</v>
+      </c>
+      <c r="C26" s="46">
+        <v>100506005.72868</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="35" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B27" s="36">
-        <v>0.05</v>
-      </c>
-      <c r="C27" s="37">
-        <f>C2*(1-(B10+B11+(1-B27)*B12+B13))</f>
-        <v>82608008.808090016</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+        <v>0.47565999999999997</v>
+      </c>
+      <c r="C27" s="47">
+        <v>365219006.73238647</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="28">
-        <f>C27/C2</f>
-        <v>0.39095500000000005</v>
+        <v>17</v>
+      </c>
+      <c r="B28" s="15">
+        <v>0.52434000000000003</v>
       </c>
       <c r="C28" s="31">
-        <f>B28*C9</f>
-        <v>300181215.10545385</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+        <v>402596253.60564172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A29" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="38">
-        <f>1-B28</f>
-        <v>0.60904499999999995</v>
-      </c>
-      <c r="C29" s="34">
-        <f>C9-C28</f>
-        <v>467634045.23257434</v>
+        <v>30</v>
+      </c>
+      <c r="B29" s="33"/>
+      <c r="C29" s="46">
+        <v>203900.8776860158</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="36">
-        <v>0.05</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B30" s="36"/>
       <c r="C30" s="37">
-        <f>C2*(1-(B10+B11+B12+(1-B30)*B13))</f>
-        <v>82592161.458240002</v>
+        <v>4660591.4899660759</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="C31" s="45">
+        <v>82608008.808090016</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="28">
-        <f>C30/C2</f>
-        <v>0.39088000000000001</v>
-      </c>
-      <c r="C31" s="31">
-        <f>B31*C9</f>
-        <v>300123628.96092844</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" s="32" t="s">
+      <c r="B32" s="38">
+        <v>0.39095500000000005</v>
+      </c>
+      <c r="C32" s="34">
+        <v>300181215.10545385</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="38">
-        <f>1-B31</f>
-        <v>0.60911999999999999</v>
-      </c>
-      <c r="C32" s="34">
-        <f>C9-C31</f>
-        <v>467691631.37709975</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="57" x14ac:dyDescent="0.45">
-      <c r="A33" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="36">
-        <v>0.1</v>
-      </c>
-      <c r="C33" s="39">
-        <f>C2*(1-(B10+B11+(1-B33)*(B12+B13)))</f>
-        <v>83498629.869660005</v>
+      <c r="B33" s="48">
+        <v>0.60904499999999995</v>
+      </c>
+      <c r="C33" s="49">
+        <v>467634045.23257434</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="40">
-        <f>C33/C2</f>
-        <v>0.39517000000000002</v>
-      </c>
-      <c r="C34" s="31">
-        <f>B34*C9</f>
-        <v>303417556.4277786</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+      <c r="B34" s="50"/>
+      <c r="C34" s="45">
+        <v>3443.3121754080057</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="41">
-        <f>1-B34</f>
-        <v>0.60482999999999998</v>
-      </c>
-      <c r="C35" s="34">
-        <f>C9-C34</f>
-        <v>464397703.91024959</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A36" s="42" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="B35" s="51"/>
+      <c r="C35" s="46">
+        <v>78704.278295040131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="39" t="s">
+        <v>20</v>
       </c>
       <c r="B36" s="15">
         <v>0.05</v>
       </c>
-      <c r="C36" s="43">
-        <f>B36*C2</f>
+      <c r="C36" s="40">
+        <v>82592161.458240002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="28">
+        <v>0.39088000000000001</v>
+      </c>
+      <c r="C37" s="52">
+        <v>300123628.96092844</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="54">
+        <v>0.60911999999999999</v>
+      </c>
+      <c r="C38" s="55">
+        <v>467691631.37709975</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="56"/>
+      <c r="C39" s="16">
+        <v>3265.8218570878503</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="56"/>
+      <c r="C40" s="16">
+        <v>74647.35673343658</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="C41" s="16">
+        <v>83498629.869660005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="54">
+        <v>0.39517000000000002</v>
+      </c>
+      <c r="C42" s="55">
+        <v>303417556.4277786</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" s="54">
+        <v>0.60482999999999998</v>
+      </c>
+      <c r="C43" s="55">
+        <v>464397703.91024959</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="56"/>
+      <c r="C44" s="16">
+        <v>13418.26806499188</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="56"/>
+      <c r="C45" s="16">
+        <v>21375649.24663296</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="56">
+        <v>0.05</v>
+      </c>
+      <c r="C46" s="16">
         <v>10564899.9</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="44">
-        <f>B36*C9</f>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="56"/>
+      <c r="C47" s="57">
         <v>38390763.016901411</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes for the presentation
</commit_message>
<xml_diff>
--- a/B_plan_data.xlsx
+++ b/B_plan_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGG\Dropbox\Github\Vestergaard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8179B2-DB77-4627-A77B-176743151046}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590A12D4-1EC7-4FD1-A4A6-B329EE78FF18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19740" yWindow="-1120" windowWidth="17600" windowHeight="18470" xr2:uid="{DAAE4708-AB0F-478A-8CE9-929A85F3F5BE}"/>
+    <workbookView xWindow="-11470" yWindow="-500" windowWidth="8810" windowHeight="17670" xr2:uid="{DAAE4708-AB0F-478A-8CE9-929A85F3F5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>ITN MOP budget</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Overall MOP 2019 budget (Africa)</t>
   </si>
   <si>
-    <t>ITN proportion</t>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
@@ -180,33 +177,39 @@
     <t>Reduce wear and tear loss by</t>
   </si>
   <si>
-    <t>Improve effectiveness by 
+    <t>ASP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of effective LLIN </t>
+  </si>
+  <si>
+    <t>Increase in value due to improved geographic coverage effectiveness</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Minimal insecticide efficacy loss</t>
+  </si>
+  <si>
+    <t>Cost of distribution</t>
+  </si>
+  <si>
+    <t>Number of children deaths prevented</t>
+  </si>
+  <si>
+    <t>Number of malaria cases prevented</t>
+  </si>
+  <si>
+    <t>% Reduction in geographic coverage need</t>
+  </si>
+  <si>
+    <t>Improve physical degradation by 
 (insecticide efficacy + wear and tear)</t>
   </si>
   <si>
-    <t>ASP</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Degradation value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-(Insecticide + wear and tear)</t>
-    </r>
+    <t>Total physical degradation loss
+(Insecticide efficacy + wear and tear)</t>
   </si>
   <si>
     <r>
@@ -227,32 +230,8 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-(LLIN lost + not used every night + minimal insecticide efficacy loss + wear and tear loss)</t>
+(LLIN lost + not used every night + minimal insecticide efficacy loss + wear and tear)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of effective LLIN </t>
-  </si>
-  <si>
-    <t>Increase in value due to improved geographic coverage effectiveness</t>
-  </si>
-  <si>
-    <t>Percentage</t>
-  </si>
-  <si>
-    <t>Minimal insecticide efficacy loss</t>
-  </si>
-  <si>
-    <t>Cost of distribution</t>
-  </si>
-  <si>
-    <t>Number of children deaths prevented</t>
-  </si>
-  <si>
-    <t>Number of malaria cases prevented</t>
-  </si>
-  <si>
-    <t>% Reduction in geographic coverage need</t>
   </si>
 </sst>
 </file>
@@ -494,7 +473,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -625,6 +604,9 @@
     <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -988,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39F588E-C6A6-449E-9F18-FF74BC1B1FFB}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1001,13 +983,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -1021,7 +1003,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="22">
@@ -1033,7 +1015,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2">
-        <v>0.71</v>
+        <v>0.7</v>
       </c>
       <c r="C4" s="23">
         <f>C3*C2</f>
@@ -1050,13 +1032,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="26">
-        <v>0.1842</v>
-      </c>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
@@ -1070,14 +1048,14 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="43" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="C8" s="3">
-        <f>(C4/0.71)*0.29</f>
-        <v>222666425.49802819</v>
+        <f>(C4/B4)*B8</f>
+        <v>233635214.93142861</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -1089,7 +1067,7 @@
       </c>
       <c r="C9" s="5">
         <f>C4+C8</f>
-        <v>767815260.33802819</v>
+        <v>778784049.77142859</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -1101,7 +1079,7 @@
       </c>
       <c r="C10" s="7">
         <f>B10*C9</f>
-        <v>94441277.021577463</v>
+        <v>95790438.121885717</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1114,12 +1092,12 @@
       </c>
       <c r="C11" s="7">
         <f>B11*C$9</f>
-        <v>330774814.15362251</v>
+        <v>335500168.64153141</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="44" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B12" s="9">
         <f>1-0.9709</f>
@@ -1127,7 +1105,7 @@
       </c>
       <c r="C12" s="7">
         <f t="shared" ref="C12:C16" si="0">B12*C$9</f>
-        <v>22343424.075836632</v>
+        <v>22662615.848348584</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -1139,7 +1117,7 @@
       </c>
       <c r="C13" s="10">
         <f t="shared" si="0"/>
-        <v>21191701.185329579</v>
+        <v>21494439.773691427</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1154,7 +1132,7 @@
     </row>
     <row r="15" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="44" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="11">
@@ -1162,9 +1140,9 @@
         <v>82300570.221000016</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B16" s="8">
         <f>B12+B13</f>
@@ -1172,12 +1150,12 @@
       </c>
       <c r="C16" s="13">
         <f t="shared" si="0"/>
-        <v>43535125.261166207</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
+        <v>44157055.622040011</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B17" s="8">
         <f>B10+B11+B12+B13</f>
@@ -1185,7 +1163,7 @@
       </c>
       <c r="C17" s="41">
         <f>B17*C$9</f>
-        <v>468751216.43636614</v>
+        <v>475447662.3854571</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -1208,7 +1186,7 @@
       </c>
       <c r="C19" s="17">
         <f>B19*C9</f>
-        <v>299064043.90166205</v>
+        <v>303336387.38597149</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1221,12 +1199,12 @@
       </c>
       <c r="C20" s="29">
         <f>C9-C19</f>
-        <v>468751216.43636614</v>
+        <v>475447662.3854571</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="19">
         <v>0.2</v>
@@ -1237,7 +1215,7 @@
     </row>
     <row r="22" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="15">
         <v>0.41410000000000002</v>
@@ -1248,7 +1226,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="33">
         <v>0.58589999999999998</v>
@@ -1257,18 +1235,18 @@
         <v>449862961.03205073</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="35" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B24" s="36"/>
       <c r="C24" s="37">
         <v>58216.824408959816</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="45">
@@ -1277,7 +1255,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" s="33">
         <v>0.2</v>
@@ -1286,9 +1264,9 @@
         <v>100506005.72868</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" s="36">
         <v>0.47565999999999997</v>
@@ -1299,7 +1277,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="15">
         <v>0.52434000000000003</v>
@@ -1308,27 +1286,27 @@
         <v>402596253.60564172</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B29" s="33"/>
       <c r="C29" s="46">
         <v>203900.8776860158</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="35" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B30" s="36"/>
       <c r="C30" s="37">
         <v>4660591.4899660759</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="15">
         <v>0.05</v>
@@ -1337,9 +1315,9 @@
         <v>82608008.808090016</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" s="38">
         <v>0.39095500000000005</v>
@@ -1350,7 +1328,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="48">
         <v>0.60904499999999995</v>
@@ -1359,18 +1337,18 @@
         <v>467634045.23257434</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B34" s="50"/>
       <c r="C34" s="45">
         <v>3443.3121754080057</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="32" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B35" s="51"/>
       <c r="C35" s="46">
@@ -1379,7 +1357,7 @@
     </row>
     <row r="36" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B36" s="15">
         <v>0.05</v>
@@ -1390,7 +1368,7 @@
     </row>
     <row r="37" spans="1:3" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B37" s="28">
         <v>0.39088000000000001</v>
@@ -1401,7 +1379,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B38" s="54">
         <v>0.60911999999999999</v>
@@ -1412,7 +1390,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="53" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B39" s="56"/>
       <c r="C39" s="16">
@@ -1421,16 +1399,16 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="53" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B40" s="56"/>
       <c r="C40" s="16">
         <v>74647.35673343658</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A41" s="53" t="s">
-        <v>21</v>
+    <row r="41" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A41" s="58" t="s">
+        <v>29</v>
       </c>
       <c r="B41" s="56">
         <v>0.1</v>
@@ -1441,7 +1419,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B42" s="54">
         <v>0.39517000000000002</v>
@@ -1452,7 +1430,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B43" s="54">
         <v>0.60482999999999998</v>
@@ -1463,7 +1441,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="53" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B44" s="56"/>
       <c r="C44" s="16">
@@ -1472,7 +1450,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="53" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B45" s="56"/>
       <c r="C45" s="16">
@@ -1481,7 +1459,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" s="53" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B46" s="56">
         <v>0.05</v>
@@ -1492,7 +1470,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="53" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B47" s="56"/>
       <c r="C47" s="57">

</xml_diff>